<commit_message>
Remapping the correct LED layout
</commit_message>
<xml_diff>
--- a/01_Pixels.xlsx
+++ b/01_Pixels.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdomoney/Projects/hackathon11fastled/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colind/Projects/ZeroOne/ZeroOne/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ver 2" sheetId="2" r:id="rId1"/>
+    <sheet name="Ver 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="image" localSheetId="0">Sheet1!$A$1:$AM$29</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$AL$29</definedName>
+    <definedName name="image" localSheetId="1">'Ver 1'!$A$1:$AM$29</definedName>
+    <definedName name="image" localSheetId="0">'Ver 2'!$A$1:$AM$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Ver 1'!$A$1:$AL$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Ver 2'!$A$1:$AL$28</definedName>
   </definedNames>
-  <calcPr calcId="150000" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="162913" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +36,52 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="image" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/cdomoney/Projects/hackathon11fastled/Utils/ImageConverter/ImageConverter/bin/Debug/image.csv" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/cdomoney/Projects/hackathon11fastled/Utils/ImageConverter/ImageConverter/bin/Debug/image.csv" comma="1">
+      <textFields count="39">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="image1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/cdomoney/Projects/hackathon11fastled/Utils/ImageConverter/ImageConverter/bin/Debug/image.csv" comma="1">
       <textFields count="39">
         <textField/>
         <textField/>
@@ -81,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -97,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,13 +171,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -140,11 +209,18 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="image" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="image" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -411,12 +487,3526 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AQ30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="42" max="42" width="12.83203125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>0</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>0</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1">
+        <v>0</v>
+      </c>
+      <c r="V1">
+        <v>0</v>
+      </c>
+      <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+      <c r="Y1">
+        <v>0</v>
+      </c>
+      <c r="Z1">
+        <v>0</v>
+      </c>
+      <c r="AA1">
+        <v>0</v>
+      </c>
+      <c r="AB1">
+        <v>0</v>
+      </c>
+      <c r="AC1">
+        <v>0</v>
+      </c>
+      <c r="AD1">
+        <v>0</v>
+      </c>
+      <c r="AE1">
+        <v>0</v>
+      </c>
+      <c r="AF1">
+        <v>0</v>
+      </c>
+      <c r="AG1">
+        <v>0</v>
+      </c>
+      <c r="AH1">
+        <v>0</v>
+      </c>
+      <c r="AI1">
+        <v>0</v>
+      </c>
+      <c r="AJ1">
+        <v>0</v>
+      </c>
+      <c r="AK1">
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <v>0</v>
+      </c>
+      <c r="AP1" s="1">
+        <f>COUNTIF(A1:AL1, "&lt;&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="AQ1">
+        <f>AP1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>1</v>
+      </c>
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
+        <v>1</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="1">
+        <f>COUNTIF(A2:AL2, "&lt;&gt;0")</f>
+        <v>23</v>
+      </c>
+      <c r="AQ2">
+        <f>AQ1+AP2</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AP3" s="1">
+        <f>COUNTIF(A3:AL3, "&lt;&gt;0")</f>
+        <v>27</v>
+      </c>
+      <c r="AQ3" s="2">
+        <f>AQ2+AP3</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>1</v>
+      </c>
+      <c r="AF4">
+        <v>1</v>
+      </c>
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4">
+        <v>1</v>
+      </c>
+      <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="1">
+        <f t="shared" ref="AP4:AP28" si="0">COUNTIF(A4:AL4, "&lt;&gt;0")</f>
+        <v>29</v>
+      </c>
+      <c r="AQ4">
+        <f>AP4</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AP5" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AQ5" s="2">
+        <f>AQ4+AP5</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6">
+        <v>1</v>
+      </c>
+      <c r="AG6">
+        <v>1</v>
+      </c>
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
+        <v>1</v>
+      </c>
+      <c r="AJ6">
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <v>1</v>
+      </c>
+      <c r="AL6">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AQ6">
+        <f>AP6</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AK7">
+        <v>1</v>
+      </c>
+      <c r="AL7">
+        <v>1</v>
+      </c>
+      <c r="AP7" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="AQ7" s="2">
+        <f>AQ6+AP7</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AQ8">
+        <f>AP8</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>1</v>
+      </c>
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
+        <v>1</v>
+      </c>
+      <c r="AJ9">
+        <v>1</v>
+      </c>
+      <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AQ9" s="3">
+        <f>AQ8+AP9</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>1</v>
+      </c>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
+        <v>1</v>
+      </c>
+      <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AP10" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ10" s="2">
+        <f>AQ9+AP10</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>1</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
+        <v>1</v>
+      </c>
+      <c r="AJ11">
+        <v>1</v>
+      </c>
+      <c r="AK11">
+        <v>1</v>
+      </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ11">
+        <f>AP11</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>1</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>1</v>
+      </c>
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
+        <v>1</v>
+      </c>
+      <c r="AJ12">
+        <v>1</v>
+      </c>
+      <c r="AK12">
+        <v>1</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AQ12" s="3">
+        <f>AQ11+AP12</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>1</v>
+      </c>
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <v>1</v>
+      </c>
+      <c r="AH13">
+        <v>1</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
+        <v>1</v>
+      </c>
+      <c r="AK13">
+        <v>1</v>
+      </c>
+      <c r="AL13">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ13" s="2">
+        <f>AQ12+AP13</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>1</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>1</v>
+      </c>
+      <c r="AH14">
+        <v>1</v>
+      </c>
+      <c r="AI14">
+        <v>1</v>
+      </c>
+      <c r="AJ14">
+        <v>1</v>
+      </c>
+      <c r="AK14">
+        <v>1</v>
+      </c>
+      <c r="AL14">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ14">
+        <f>AP14</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>1</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>1</v>
+      </c>
+      <c r="AH15">
+        <v>1</v>
+      </c>
+      <c r="AI15">
+        <v>1</v>
+      </c>
+      <c r="AJ15">
+        <v>1</v>
+      </c>
+      <c r="AK15">
+        <v>1</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ15" s="3">
+        <f>AQ14+AP15</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>1</v>
+      </c>
+      <c r="AH16">
+        <v>1</v>
+      </c>
+      <c r="AI16">
+        <v>1</v>
+      </c>
+      <c r="AJ16">
+        <v>1</v>
+      </c>
+      <c r="AK16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AP16" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ16" s="2">
+        <f>AQ15+AP16</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>1</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>1</v>
+      </c>
+      <c r="AH17">
+        <v>1</v>
+      </c>
+      <c r="AI17">
+        <v>1</v>
+      </c>
+      <c r="AJ17">
+        <v>1</v>
+      </c>
+      <c r="AK17">
+        <v>1</v>
+      </c>
+      <c r="AL17">
+        <v>1</v>
+      </c>
+      <c r="AP17" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ17">
+        <f>AP17</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>1</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
+      <c r="AK18">
+        <v>1</v>
+      </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AP18" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ18" s="3">
+        <f>AQ17+AP18</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
+        <v>1</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
+      </c>
+      <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AP19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="AQ19" s="2">
+        <f>AQ18+AP19</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>1</v>
+      </c>
+      <c r="AI20">
+        <v>1</v>
+      </c>
+      <c r="AJ20">
+        <v>1</v>
+      </c>
+      <c r="AK20">
+        <v>1</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AQ20">
+        <f>AP20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>1</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>1</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>1</v>
+      </c>
+      <c r="AK21">
+        <v>1</v>
+      </c>
+      <c r="AL21">
+        <v>1</v>
+      </c>
+      <c r="AP21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AQ21" s="3">
+        <f>AQ20+AP21</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>0</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>1</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>1</v>
+      </c>
+      <c r="AK22">
+        <v>1</v>
+      </c>
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AP22" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AQ22" s="2">
+        <f>AQ21+AP22</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>1</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>1</v>
+      </c>
+      <c r="AI23">
+        <v>1</v>
+      </c>
+      <c r="AJ23">
+        <v>1</v>
+      </c>
+      <c r="AK23">
+        <v>1</v>
+      </c>
+      <c r="AL23">
+        <v>1</v>
+      </c>
+      <c r="AP23" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AQ23">
+        <f>AP23</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>1</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>1</v>
+      </c>
+      <c r="AI24">
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <v>1</v>
+      </c>
+      <c r="AK24">
+        <v>1</v>
+      </c>
+      <c r="AL24">
+        <v>1</v>
+      </c>
+      <c r="AP24" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AQ24" s="2">
+        <f>AQ23+AP24</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>1</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>1</v>
+      </c>
+      <c r="AI25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>1</v>
+      </c>
+      <c r="AK25">
+        <v>1</v>
+      </c>
+      <c r="AL25">
+        <v>1</v>
+      </c>
+      <c r="AP25" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AQ25">
+        <f>AP25</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <v>0</v>
+      </c>
+      <c r="AG26">
+        <v>1</v>
+      </c>
+      <c r="AH26">
+        <v>1</v>
+      </c>
+      <c r="AI26">
+        <v>1</v>
+      </c>
+      <c r="AJ26">
+        <v>1</v>
+      </c>
+      <c r="AK26">
+        <v>1</v>
+      </c>
+      <c r="AL26">
+        <v>1</v>
+      </c>
+      <c r="AP26" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="AQ26" s="2">
+        <f>AQ25+AP26</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>0</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>1</v>
+      </c>
+      <c r="AI27">
+        <v>1</v>
+      </c>
+      <c r="AJ27">
+        <v>1</v>
+      </c>
+      <c r="AK27">
+        <v>1</v>
+      </c>
+      <c r="AL27">
+        <v>1</v>
+      </c>
+      <c r="AP27" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="AQ27">
+        <f>AP27</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>0</v>
+      </c>
+      <c r="W28">
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28">
+        <v>0</v>
+      </c>
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>0</v>
+      </c>
+      <c r="AF28">
+        <v>0</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
+        <v>1</v>
+      </c>
+      <c r="AJ28">
+        <v>1</v>
+      </c>
+      <c r="AK28">
+        <v>1</v>
+      </c>
+      <c r="AL28">
+        <v>1</v>
+      </c>
+      <c r="AP28" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="AQ28" s="2">
+        <f>AQ27+AP28</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AP30" s="1">
+        <f>SUM(AP1:AP29)</f>
+        <v>592</v>
+      </c>
+      <c r="AQ30">
+        <f>AQ3+AQ5+AQ7+AQ10+AQ13+AQ16+AQ19+AQ22+AQ24+AQ26+AQ28</f>
+        <v>592</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:AO1048576 AR1:XFD1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0.1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="AQ25 AQ27 AQ23 AQ20 AQ17 AQ14 AQ11 AQ8 AQ6 AQ4" formula="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AL29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Getting much of the Python GUI stuff done on the PC side, plus the LEDs
</commit_message>
<xml_diff>
--- a/01_Pixels.xlsx
+++ b/01_Pixels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="-22560" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="-22560" windowWidth="33600" windowHeight="20540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ver 2" sheetId="2" r:id="rId1"/>
@@ -183,7 +183,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -525,8 +553,8 @@
   </sheetPr>
   <dimension ref="A1:AR30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AR30" sqref="AR30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AL28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4064,16 +4092,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AL28">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>22</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7466,7 +7494,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7480,8 +7508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AS28" sqref="AS28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:AL28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7521,25 +7549,25 @@
         <v>0</v>
       </c>
       <c r="L1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="R1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S1">
         <v>0</v>
@@ -7628,16 +7656,16 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -7655,16 +7683,16 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -7688,34 +7716,34 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AD2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AE2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AF2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AG2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AI2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AJ2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AK2">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AL2">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.2">
@@ -7738,13 +7766,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -7780,13 +7808,13 @@
         <v>1</v>
       </c>
       <c r="U3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -7804,7 +7832,7 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AD3">
         <v>2</v>
@@ -7831,7 +7859,7 @@
         <v>2</v>
       </c>
       <c r="AL3">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.2">
@@ -7851,10 +7879,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -7902,10 +7930,10 @@
         <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y4">
         <v>0</v>
@@ -7920,7 +7948,7 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AD4">
         <v>2</v>
@@ -7947,7 +7975,7 @@
         <v>2</v>
       </c>
       <c r="AL4">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.2">
@@ -7964,10 +7992,10 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -8021,10 +8049,10 @@
         <v>1</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y5">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -8036,7 +8064,7 @@
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AD5">
         <v>2</v>
@@ -8063,7 +8091,7 @@
         <v>2</v>
       </c>
       <c r="AL5">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.2">
@@ -8077,10 +8105,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -8098,31 +8126,31 @@
         <v>1</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T6">
         <v>1</v>
@@ -8140,10 +8168,10 @@
         <v>1</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Z6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -8152,19 +8180,19 @@
         <v>0</v>
       </c>
       <c r="AC6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AD6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AE6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AF6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AG6">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH6">
         <v>2</v>
@@ -8179,7 +8207,7 @@
         <v>2</v>
       </c>
       <c r="AL6">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
@@ -8193,7 +8221,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -8208,13 +8236,13 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -8238,13 +8266,13 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -8259,7 +8287,7 @@
         <v>1</v>
       </c>
       <c r="Z7">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -8280,7 +8308,7 @@
         <v>0</v>
       </c>
       <c r="AG7">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH7">
         <v>2</v>
@@ -8295,7 +8323,7 @@
         <v>2</v>
       </c>
       <c r="AL7">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.2">
@@ -8306,10 +8334,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -8321,10 +8349,10 @@
         <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -8360,10 +8388,10 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W8">
         <v>1</v>
@@ -8375,10 +8403,10 @@
         <v>1</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AB8">
         <v>0</v>
@@ -8396,7 +8424,7 @@
         <v>0</v>
       </c>
       <c r="AG8">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH8">
         <v>2</v>
@@ -8411,7 +8439,7 @@
         <v>2</v>
       </c>
       <c r="AL8">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.2">
@@ -8419,10 +8447,10 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -8434,10 +8462,10 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -8479,10 +8507,10 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -8494,10 +8522,10 @@
         <v>1</v>
       </c>
       <c r="AA9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AB9">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC9">
         <v>0</v>
@@ -8512,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="AG9">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH9">
         <v>2</v>
@@ -8527,7 +8555,7 @@
         <v>2</v>
       </c>
       <c r="AL9">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.2">
@@ -8535,7 +8563,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -8550,7 +8578,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -8598,7 +8626,7 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X10">
         <v>1</v>
@@ -8613,7 +8641,7 @@
         <v>1</v>
       </c>
       <c r="AB10">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC10">
         <v>0</v>
@@ -8628,7 +8656,7 @@
         <v>0</v>
       </c>
       <c r="AG10">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH10">
         <v>2</v>
@@ -8643,7 +8671,7 @@
         <v>2</v>
       </c>
       <c r="AL10">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.2">
@@ -8651,7 +8679,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -8663,10 +8691,10 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -8714,10 +8742,10 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y11">
         <v>1</v>
@@ -8729,7 +8757,7 @@
         <v>1</v>
       </c>
       <c r="AB11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC11">
         <v>0</v>
@@ -8744,7 +8772,7 @@
         <v>0</v>
       </c>
       <c r="AG11">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH11">
         <v>2</v>
@@ -8759,15 +8787,15 @@
         <v>2</v>
       </c>
       <c r="AL11">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -8779,7 +8807,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -8833,7 +8861,7 @@
         <v>0</v>
       </c>
       <c r="X12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y12">
         <v>1</v>
@@ -8845,10 +8873,10 @@
         <v>1</v>
       </c>
       <c r="AB12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC12">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -8860,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="AG12">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH12">
         <v>2</v>
@@ -8875,12 +8903,12 @@
         <v>2</v>
       </c>
       <c r="AL12">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -8895,7 +8923,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -8949,7 +8977,7 @@
         <v>0</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y13">
         <v>1</v>
@@ -8964,7 +8992,7 @@
         <v>1</v>
       </c>
       <c r="AC13">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -8976,7 +9004,7 @@
         <v>0</v>
       </c>
       <c r="AG13">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH13">
         <v>2</v>
@@ -8991,12 +9019,12 @@
         <v>2</v>
       </c>
       <c r="AL13">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -9011,7 +9039,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -9065,7 +9093,7 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y14">
         <v>1</v>
@@ -9080,7 +9108,7 @@
         <v>1</v>
       </c>
       <c r="AC14">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -9092,7 +9120,7 @@
         <v>0</v>
       </c>
       <c r="AG14">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH14">
         <v>2</v>
@@ -9107,12 +9135,12 @@
         <v>2</v>
       </c>
       <c r="AL14">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -9127,7 +9155,7 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -9181,7 +9209,7 @@
         <v>0</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y15">
         <v>1</v>
@@ -9196,7 +9224,7 @@
         <v>1</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -9208,7 +9236,7 @@
         <v>0</v>
       </c>
       <c r="AG15">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH15">
         <v>2</v>
@@ -9223,12 +9251,12 @@
         <v>2</v>
       </c>
       <c r="AL15">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -9243,7 +9271,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -9297,7 +9325,7 @@
         <v>0</v>
       </c>
       <c r="X16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y16">
         <v>1</v>
@@ -9312,7 +9340,7 @@
         <v>1</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -9324,7 +9352,7 @@
         <v>0</v>
       </c>
       <c r="AG16">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH16">
         <v>2</v>
@@ -9339,15 +9367,15 @@
         <v>2</v>
       </c>
       <c r="AL16">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -9359,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -9413,7 +9441,7 @@
         <v>0</v>
       </c>
       <c r="X17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y17">
         <v>1</v>
@@ -9425,10 +9453,10 @@
         <v>1</v>
       </c>
       <c r="AB17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC17">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AD17">
         <v>0</v>
@@ -9440,7 +9468,7 @@
         <v>0</v>
       </c>
       <c r="AG17">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH17">
         <v>2</v>
@@ -9455,7 +9483,7 @@
         <v>2</v>
       </c>
       <c r="AL17">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.2">
@@ -9463,7 +9491,7 @@
         <v>0</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -9475,10 +9503,10 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -9526,10 +9554,10 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y18">
         <v>1</v>
@@ -9541,7 +9569,7 @@
         <v>1</v>
       </c>
       <c r="AB18">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC18">
         <v>0</v>
@@ -9556,7 +9584,7 @@
         <v>0</v>
       </c>
       <c r="AG18">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH18">
         <v>2</v>
@@ -9571,7 +9599,7 @@
         <v>2</v>
       </c>
       <c r="AL18">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.2">
@@ -9579,7 +9607,7 @@
         <v>0</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -9594,7 +9622,7 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -9642,7 +9670,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X19">
         <v>1</v>
@@ -9657,7 +9685,7 @@
         <v>1</v>
       </c>
       <c r="AB19">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC19">
         <v>0</v>
@@ -9672,7 +9700,7 @@
         <v>0</v>
       </c>
       <c r="AG19">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH19">
         <v>2</v>
@@ -9687,7 +9715,7 @@
         <v>2</v>
       </c>
       <c r="AL19">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.2">
@@ -9695,10 +9723,10 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -9710,10 +9738,10 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -9755,10 +9783,10 @@
         <v>0</v>
       </c>
       <c r="V20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X20">
         <v>1</v>
@@ -9773,7 +9801,7 @@
         <v>1</v>
       </c>
       <c r="AB20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AC20">
         <v>0</v>
@@ -9788,7 +9816,7 @@
         <v>0</v>
       </c>
       <c r="AG20">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH20">
         <v>2</v>
@@ -9803,7 +9831,7 @@
         <v>2</v>
       </c>
       <c r="AL20">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.2">
@@ -9814,7 +9842,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -9829,10 +9857,10 @@
         <v>1</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -9868,10 +9896,10 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W21">
         <v>1</v>
@@ -9883,10 +9911,10 @@
         <v>1</v>
       </c>
       <c r="Z21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AB21">
         <v>0</v>
@@ -9904,7 +9932,7 @@
         <v>0</v>
       </c>
       <c r="AG21">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH21">
         <v>2</v>
@@ -9919,7 +9947,7 @@
         <v>2</v>
       </c>
       <c r="AL21">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.2">
@@ -9930,10 +9958,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -9948,13 +9976,13 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -9978,13 +10006,13 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="U22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V22">
         <v>1</v>
@@ -9999,7 +10027,7 @@
         <v>1</v>
       </c>
       <c r="Z22">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA22">
         <v>0</v>
@@ -10020,7 +10048,7 @@
         <v>0</v>
       </c>
       <c r="AG22">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH22">
         <v>2</v>
@@ -10035,7 +10063,7 @@
         <v>2</v>
       </c>
       <c r="AL22">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.2">
@@ -10049,10 +10077,10 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -10070,31 +10098,31 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="R23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T23">
         <v>1</v>
@@ -10112,10 +10140,10 @@
         <v>1</v>
       </c>
       <c r="Y23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Z23">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -10136,7 +10164,7 @@
         <v>0</v>
       </c>
       <c r="AG23">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH23">
         <v>2</v>
@@ -10151,7 +10179,7 @@
         <v>2</v>
       </c>
       <c r="AL23">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.2">
@@ -10168,10 +10196,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -10225,10 +10253,10 @@
         <v>1</v>
       </c>
       <c r="X24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y24">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -10252,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="AG24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH24">
         <v>2</v>
@@ -10267,7 +10295,7 @@
         <v>2</v>
       </c>
       <c r="AL24">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.2">
@@ -10287,10 +10315,10 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -10338,10 +10366,10 @@
         <v>1</v>
       </c>
       <c r="W25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Y25">
         <v>0</v>
@@ -10368,7 +10396,7 @@
         <v>0</v>
       </c>
       <c r="AG25">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH25">
         <v>2</v>
@@ -10383,7 +10411,7 @@
         <v>2</v>
       </c>
       <c r="AL25">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.2">
@@ -10406,13 +10434,13 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J26">
         <v>1</v>
@@ -10448,13 +10476,13 @@
         <v>1</v>
       </c>
       <c r="U26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="W26">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="X26">
         <v>0</v>
@@ -10484,7 +10512,7 @@
         <v>0</v>
       </c>
       <c r="AG26">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH26">
         <v>2</v>
@@ -10499,7 +10527,7 @@
         <v>2</v>
       </c>
       <c r="AL26">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.2">
@@ -10528,16 +10556,16 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -10555,16 +10583,16 @@
         <v>1</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="T27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="U27">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="V27">
         <v>0</v>
@@ -10600,7 +10628,7 @@
         <v>0</v>
       </c>
       <c r="AG27">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH27">
         <v>2</v>
@@ -10615,7 +10643,7 @@
         <v>2</v>
       </c>
       <c r="AL27">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.2">
@@ -10653,25 +10681,25 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="O28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="R28">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="S28">
         <v>0</v>
@@ -10716,31 +10744,37 @@
         <v>0</v>
       </c>
       <c r="AG28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AH28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AI28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AJ28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AK28">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="AL28">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AL28">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="2">
-      <formula>NOT(ISERROR(SEARCH("2",A1)))</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>22</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started work on converting the '01' pixel shape to a Py array
</commit_message>
<xml_diff>
--- a/01_Pixels.xlsx
+++ b/01_Pixels.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -183,11 +183,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -201,28 +208,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -239,7 +225,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -253,14 +246,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
+          <bgColor theme="4" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4092,17 +4078,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AL28">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>22</formula>
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>1</formula>
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>22</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="1"/>
@@ -7494,7 +7480,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7508,9 +7494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AL28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -10764,16 +10748,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AL28">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>22</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>